<commit_message>
Report Component Finished - Changed Validation So 1000 Rounds Are Tested NOT 15
</commit_message>
<xml_diff>
--- a/Validation.xlsx
+++ b/Validation.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\UNI\UNI YR 3\SEM 2\CITS3001\GITHUB\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ryan\Documents\UNI\UNI YR 3\SEM 2\CITS3001\PROJECT 3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3E122E9-8C83-4828-B963-6D44FE387146}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F67A15D1-0697-47B1-88DD-30CB919D8BB3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" activeTab="3" xr2:uid="{DC6A9364-D65F-4265-98B6-F123AC9CA00D}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6590" firstSheet="1" activeTab="3" xr2:uid="{DC6A9364-D65F-4265-98B6-F123AC9CA00D}"/>
   </bookViews>
   <sheets>
     <sheet name="CONSERVATIVE" sheetId="1" r:id="rId1"/>
     <sheet name="ADVANCED" sheetId="2" r:id="rId2"/>
     <sheet name="BASIC" sheetId="5" r:id="rId3"/>
-    <sheet name="BAR GRAPH" sheetId="4" r:id="rId4"/>
+    <sheet name="BAR GRAPH 15 ROUNDS" sheetId="4" r:id="rId4"/>
     <sheet name="ALL 3" sheetId="3" r:id="rId5"/>
   </sheets>
   <calcPr calcId="162913"/>
@@ -1524,7 +1524,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-AU" baseline="0"/>
-              <a:t> Scores For Three Different Agents Playing Hanabi</a:t>
+              <a:t> Scores For Three Different Agents Playing Hanabi Across 1000 Games</a:t>
             </a:r>
             <a:endParaRPr lang="en-AU"/>
           </a:p>
@@ -1591,7 +1591,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -1660,7 +1660,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'BAR GRAPH'!$A$4:$A$6</c:f>
+              <c:f>'BAR GRAPH 15 ROUNDS'!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1677,18 +1677,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BAR GRAPH'!$B$4:$B$6</c:f>
+              <c:f>'BAR GRAPH 15 ROUNDS'!$B$4:$B$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.4</c:v>
+                  <c:v>7.8150000000000004</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.73</c:v>
+                  <c:v>12.752000000000001</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.33</c:v>
+                  <c:v>12.385999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1724,7 +1724,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -1793,7 +1793,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'BAR GRAPH'!$A$4:$A$6</c:f>
+              <c:f>'BAR GRAPH 15 ROUNDS'!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1810,18 +1810,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BAR GRAPH'!$C$4:$C$6</c:f>
+              <c:f>'BAR GRAPH 15 ROUNDS'!$C$4:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.23</c:v>
+                  <c:v>7.2430000000000003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>13.8</c:v>
+                  <c:v>13.615</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.2</c:v>
+                  <c:v>13.362</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1935,7 +1935,7 @@
           </c:errBars>
           <c:cat>
             <c:strRef>
-              <c:f>'BAR GRAPH'!$A$4:$A$6</c:f>
+              <c:f>'BAR GRAPH 15 ROUNDS'!$A$4:$A$6</c:f>
               <c:strCache>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
@@ -1952,18 +1952,18 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'BAR GRAPH'!$D$4:$D$6</c:f>
+              <c:f>'BAR GRAPH 15 ROUNDS'!$D$4:$D$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>8.4</c:v>
+                  <c:v>6.3289999999999997</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.33</c:v>
+                  <c:v>12.256</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.13</c:v>
+                  <c:v>12.055999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5151,16 +5151,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>4</xdr:col>
-      <xdr:colOff>238125</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>168275</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>7937</xdr:rowOff>
+      <xdr:rowOff>23812</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>473075</xdr:colOff>
       <xdr:row>15</xdr:row>
-      <xdr:rowOff>128587</xdr:rowOff>
+      <xdr:rowOff>144462</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6710,7 +6710,7 @@
   <dimension ref="A3:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M15" sqref="M15"/>
+      <selection activeCell="A3" sqref="A3:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -6737,13 +6737,13 @@
         <v>13</v>
       </c>
       <c r="B4">
-        <v>8.4</v>
+        <v>7.8150000000000004</v>
       </c>
       <c r="C4">
-        <v>7.23</v>
+        <v>7.2430000000000003</v>
       </c>
       <c r="D4">
-        <v>8.4</v>
+        <v>6.3289999999999997</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.75">
@@ -6751,13 +6751,13 @@
         <v>14</v>
       </c>
       <c r="B5">
-        <v>12.73</v>
+        <v>12.752000000000001</v>
       </c>
       <c r="C5">
-        <v>13.8</v>
+        <v>13.615</v>
       </c>
       <c r="D5" s="3">
-        <v>12.33</v>
+        <v>12.256</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.75">
@@ -6765,13 +6765,13 @@
         <v>15</v>
       </c>
       <c r="B6">
-        <v>12.33</v>
+        <v>12.385999999999999</v>
       </c>
       <c r="C6">
-        <v>13.2</v>
+        <v>13.362</v>
       </c>
       <c r="D6">
-        <v>13.13</v>
+        <v>12.055999999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>